<commit_message>
add two sablon and some date unfold
</commit_message>
<xml_diff>
--- a/contracts-list.xlsx
+++ b/contracts-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t xml:space="preserve">FIRST_NAME</t>
   </si>
@@ -67,7 +67,40 @@
     <t xml:space="preserve">PASSPORT_NUMBER</t>
   </si>
   <si>
+    <t xml:space="preserve">PASSPORT_VALID_DATE</t>
+  </si>
+  <si>
     <t xml:space="preserve">TART_ENG_SZAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_ISZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_HSZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_TELEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_KZTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_KZTER_JEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_HAZSZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_EPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_LH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZH_AJTO</t>
   </si>
   <si>
     <t xml:space="preserve">ER_FIRST_NAME</t>
@@ -164,9 +197,30 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">2026.01.01</t>
+  </si>
+  <si>
     <t xml:space="preserve">N7236472</t>
   </si>
   <si>
+    <t xml:space="preserve">Budapest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orlay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.em</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2/a</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAN</t>
   </si>
   <si>
@@ -206,6 +260,9 @@
     <t xml:space="preserve">1104 Budapest Gyömrői út</t>
   </si>
   <si>
+    <t xml:space="preserve">2026.01.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">N7236473</t>
   </si>
   <si>
@@ -239,6 +296,9 @@
     <t xml:space="preserve">1105 Budapest Gyömrői út</t>
   </si>
   <si>
+    <t xml:space="preserve">2026.01.03</t>
+  </si>
+  <si>
     <t xml:space="preserve">N7236474</t>
   </si>
   <si>
@@ -275,6 +335,9 @@
     <t xml:space="preserve">1106 Budapest Gyömrői út</t>
   </si>
   <si>
+    <t xml:space="preserve">2026.01.04</t>
+  </si>
+  <si>
     <t xml:space="preserve">N7236475</t>
   </si>
   <si>
@@ -306,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">1107 Budapest Gyömrői út</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026.01.05</t>
   </si>
   <si>
     <t xml:space="preserve">N7236476</t>
@@ -681,10 +747,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W101"/>
+  <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA3" activeCellId="0" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,14 +764,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="32.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="40.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="20.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="38.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="18" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="20.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="38.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="16.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="19.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,369 +820,487 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4"/>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>4532</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="O2" s="5" t="n">
         <v>324234234</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="12" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <v>1113</v>
+      </c>
+      <c r="S2" s="5" t="n">
+        <v>5463</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="12" t="n">
         <v>1413</v>
       </c>
-      <c r="W2" s="12"/>
+      <c r="AH2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>4533</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="O3" s="5" t="n">
         <v>324234235</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="12" t="n">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG3" s="12" t="n">
         <v>1413</v>
       </c>
-      <c r="W3" s="12"/>
+      <c r="AH3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>4534</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="O4" s="5" t="n">
         <v>324234236</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="12" t="n">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG4" s="12" t="n">
         <v>1413</v>
       </c>
-      <c r="W4" s="12"/>
+      <c r="AH4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>4535</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="O5" s="5" t="n">
         <v>324234237</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="V5" s="12" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG5" s="12" t="n">
         <v>1413</v>
       </c>
-      <c r="W5" s="12"/>
+      <c r="AH5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>4536</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="O6" s="5" t="n">
         <v>324234238</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T6" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" s="12" t="n">
+        <v>103</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG6" s="12" t="n">
         <v>1413</v>
       </c>
-      <c r="W6" s="12"/>
+      <c r="AH6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
@@ -1135,13 +1319,24 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -1160,13 +1355,24 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
@@ -1185,13 +1391,24 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
@@ -1210,13 +1427,24 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
@@ -1235,13 +1463,24 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
@@ -1260,13 +1499,24 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
@@ -1285,13 +1535,24 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
@@ -1310,13 +1571,24 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
@@ -1335,13 +1607,24 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
@@ -1360,13 +1643,24 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
@@ -1385,13 +1679,24 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
@@ -1410,13 +1715,24 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="8"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
@@ -1435,13 +1751,24 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
@@ -1460,13 +1787,24 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
@@ -1485,13 +1823,24 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
@@ -1510,13 +1859,24 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
@@ -1535,13 +1895,24 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
@@ -1560,13 +1931,24 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
@@ -1585,13 +1967,24 @@
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
@@ -1610,13 +2003,24 @@
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
@@ -1635,13 +2039,24 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="8"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
@@ -1660,13 +2075,24 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="8"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
@@ -1685,13 +2111,24 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="8"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
@@ -1710,13 +2147,24 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="8"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
@@ -1735,13 +2183,24 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="8"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
@@ -1760,13 +2219,24 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
@@ -1785,13 +2255,24 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="8"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9"/>
+      <c r="AF33" s="9"/>
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
@@ -1810,13 +2291,24 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="8"/>
+      <c r="AC34" s="9"/>
+      <c r="AD34" s="9"/>
+      <c r="AE34" s="9"/>
+      <c r="AF34" s="9"/>
+      <c r="AG34" s="9"/>
+      <c r="AH34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
@@ -1835,13 +2327,24 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="8"/>
+      <c r="AC35" s="9"/>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="9"/>
+      <c r="AG35" s="9"/>
+      <c r="AH35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
@@ -1860,13 +2363,24 @@
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="8"/>
+      <c r="AC36" s="9"/>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="9"/>
+      <c r="AF36" s="9"/>
+      <c r="AG36" s="9"/>
+      <c r="AH36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
@@ -1885,13 +2399,24 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="8"/>
+      <c r="AC37" s="9"/>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="9"/>
+      <c r="AF37" s="9"/>
+      <c r="AG37" s="9"/>
+      <c r="AH37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
@@ -1910,13 +2435,24 @@
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="8"/>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9"/>
+      <c r="AF38" s="9"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
@@ -1935,13 +2471,24 @@
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="8"/>
+      <c r="AC39" s="9"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
@@ -1960,13 +2507,24 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
-      <c r="U40" s="9"/>
-      <c r="V40" s="9"/>
-      <c r="W40" s="9"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="8"/>
+      <c r="AC40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+      <c r="AG40" s="9"/>
+      <c r="AH40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
@@ -1985,13 +2543,24 @@
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-      <c r="U41" s="9"/>
-      <c r="V41" s="9"/>
-      <c r="W41" s="9"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="8"/>
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="9"/>
+      <c r="AF41" s="9"/>
+      <c r="AG41" s="9"/>
+      <c r="AH41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
@@ -2010,13 +2579,24 @@
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="9"/>
-      <c r="U42" s="9"/>
-      <c r="V42" s="9"/>
-      <c r="W42" s="9"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="8"/>
+      <c r="AC42" s="9"/>
+      <c r="AD42" s="9"/>
+      <c r="AE42" s="9"/>
+      <c r="AF42" s="9"/>
+      <c r="AG42" s="9"/>
+      <c r="AH42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
@@ -2035,13 +2615,24 @@
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
-      <c r="W43" s="9"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="8"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="9"/>
+      <c r="AG43" s="9"/>
+      <c r="AH43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
@@ -2060,13 +2651,24 @@
       <c r="N44" s="5"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="8"/>
+      <c r="AC44" s="9"/>
+      <c r="AD44" s="9"/>
+      <c r="AE44" s="9"/>
+      <c r="AF44" s="9"/>
+      <c r="AG44" s="9"/>
+      <c r="AH44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
@@ -2085,13 +2687,24 @@
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="9"/>
-      <c r="U45" s="9"/>
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="8"/>
+      <c r="AC45" s="9"/>
+      <c r="AD45" s="9"/>
+      <c r="AE45" s="9"/>
+      <c r="AF45" s="9"/>
+      <c r="AG45" s="9"/>
+      <c r="AH45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
@@ -2110,13 +2723,24 @@
       <c r="N46" s="5"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="9"/>
+      <c r="AD46" s="9"/>
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="9"/>
+      <c r="AG46" s="9"/>
+      <c r="AH46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
@@ -2135,13 +2759,24 @@
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="9"/>
+      <c r="AG47" s="9"/>
+      <c r="AH47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
@@ -2160,13 +2795,24 @@
       <c r="N48" s="5"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
-      <c r="W48" s="9"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="8"/>
+      <c r="AC48" s="9"/>
+      <c r="AD48" s="9"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
+      <c r="AG48" s="9"/>
+      <c r="AH48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
@@ -2185,13 +2831,24 @@
       <c r="N49" s="5"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="8"/>
+      <c r="AC49" s="9"/>
+      <c r="AD49" s="9"/>
+      <c r="AE49" s="9"/>
+      <c r="AF49" s="9"/>
+      <c r="AG49" s="9"/>
+      <c r="AH49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
@@ -2210,13 +2867,24 @@
       <c r="N50" s="5"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="9"/>
-      <c r="T50" s="9"/>
-      <c r="U50" s="9"/>
-      <c r="V50" s="9"/>
-      <c r="W50" s="9"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="8"/>
+      <c r="AC50" s="9"/>
+      <c r="AD50" s="9"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="9"/>
+      <c r="AH50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
@@ -2235,13 +2903,24 @@
       <c r="N51" s="5"/>
       <c r="O51" s="5"/>
       <c r="P51" s="5"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="9"/>
-      <c r="S51" s="9"/>
-      <c r="T51" s="9"/>
-      <c r="U51" s="9"/>
-      <c r="V51" s="9"/>
-      <c r="W51" s="9"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="5"/>
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="8"/>
+      <c r="AC51" s="9"/>
+      <c r="AD51" s="9"/>
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="9"/>
+      <c r="AG51" s="9"/>
+      <c r="AH51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
@@ -2260,13 +2939,24 @@
       <c r="N52" s="5"/>
       <c r="O52" s="5"/>
       <c r="P52" s="5"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="9"/>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-      <c r="V52" s="9"/>
-      <c r="W52" s="9"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="5"/>
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="9"/>
+      <c r="AD52" s="9"/>
+      <c r="AE52" s="9"/>
+      <c r="AF52" s="9"/>
+      <c r="AG52" s="9"/>
+      <c r="AH52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
@@ -2285,13 +2975,24 @@
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
       <c r="P53" s="5"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="9"/>
-      <c r="T53" s="9"/>
-      <c r="U53" s="9"/>
-      <c r="V53" s="9"/>
-      <c r="W53" s="9"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="8"/>
+      <c r="AC53" s="9"/>
+      <c r="AD53" s="9"/>
+      <c r="AE53" s="9"/>
+      <c r="AF53" s="9"/>
+      <c r="AG53" s="9"/>
+      <c r="AH53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
@@ -2310,13 +3011,24 @@
       <c r="N54" s="5"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
-      <c r="Q54" s="8"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
-      <c r="U54" s="9"/>
-      <c r="V54" s="9"/>
-      <c r="W54" s="9"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="8"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
@@ -2335,13 +3047,24 @@
       <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="9"/>
-      <c r="S55" s="9"/>
-      <c r="T55" s="9"/>
-      <c r="U55" s="9"/>
-      <c r="V55" s="9"/>
-      <c r="W55" s="9"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="5"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5"/>
@@ -2360,13 +3083,24 @@
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="Q56" s="8"/>
-      <c r="R56" s="9"/>
-      <c r="S56" s="9"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="8"/>
+      <c r="AC56" s="9"/>
+      <c r="AD56" s="9"/>
+      <c r="AE56" s="9"/>
+      <c r="AF56" s="9"/>
+      <c r="AG56" s="9"/>
+      <c r="AH56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
@@ -2385,13 +3119,24 @@
       <c r="N57" s="5"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="9"/>
-      <c r="S57" s="9"/>
-      <c r="T57" s="9"/>
-      <c r="U57" s="9"/>
-      <c r="V57" s="9"/>
-      <c r="W57" s="9"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="5"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="5"/>
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="8"/>
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="9"/>
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="9"/>
+      <c r="AG57" s="9"/>
+      <c r="AH57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5"/>
@@ -2410,13 +3155,24 @@
       <c r="N58" s="5"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
-      <c r="Q58" s="8"/>
-      <c r="R58" s="9"/>
-      <c r="S58" s="9"/>
-      <c r="T58" s="9"/>
-      <c r="U58" s="9"/>
-      <c r="V58" s="9"/>
-      <c r="W58" s="9"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="8"/>
+      <c r="AC58" s="9"/>
+      <c r="AD58" s="9"/>
+      <c r="AE58" s="9"/>
+      <c r="AF58" s="9"/>
+      <c r="AG58" s="9"/>
+      <c r="AH58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
@@ -2435,13 +3191,24 @@
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
-      <c r="Q59" s="8"/>
-      <c r="R59" s="9"/>
-      <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="5"/>
+      <c r="AB59" s="8"/>
+      <c r="AC59" s="9"/>
+      <c r="AD59" s="9"/>
+      <c r="AE59" s="9"/>
+      <c r="AF59" s="9"/>
+      <c r="AG59" s="9"/>
+      <c r="AH59" s="9"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
@@ -2460,13 +3227,24 @@
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="9"/>
-      <c r="S60" s="9"/>
-      <c r="T60" s="9"/>
-      <c r="U60" s="9"/>
-      <c r="V60" s="9"/>
-      <c r="W60" s="9"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="5"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="5"/>
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="8"/>
+      <c r="AC60" s="9"/>
+      <c r="AD60" s="9"/>
+      <c r="AE60" s="9"/>
+      <c r="AF60" s="9"/>
+      <c r="AG60" s="9"/>
+      <c r="AH60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
@@ -2485,13 +3263,24 @@
       <c r="N61" s="5"/>
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
-      <c r="Q61" s="8"/>
-      <c r="R61" s="9"/>
-      <c r="S61" s="9"/>
-      <c r="T61" s="9"/>
-      <c r="U61" s="9"/>
-      <c r="V61" s="9"/>
-      <c r="W61" s="9"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+      <c r="AA61" s="5"/>
+      <c r="AB61" s="8"/>
+      <c r="AC61" s="9"/>
+      <c r="AD61" s="9"/>
+      <c r="AE61" s="9"/>
+      <c r="AF61" s="9"/>
+      <c r="AG61" s="9"/>
+      <c r="AH61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5"/>
@@ -2510,13 +3299,24 @@
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="9"/>
-      <c r="S62" s="9"/>
-      <c r="T62" s="9"/>
-      <c r="U62" s="9"/>
-      <c r="V62" s="9"/>
-      <c r="W62" s="9"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="5"/>
+      <c r="AB62" s="8"/>
+      <c r="AC62" s="9"/>
+      <c r="AD62" s="9"/>
+      <c r="AE62" s="9"/>
+      <c r="AF62" s="9"/>
+      <c r="AG62" s="9"/>
+      <c r="AH62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5"/>
@@ -2535,13 +3335,24 @@
       <c r="N63" s="5"/>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
-      <c r="Q63" s="8"/>
-      <c r="R63" s="9"/>
-      <c r="S63" s="9"/>
-      <c r="T63" s="9"/>
-      <c r="U63" s="9"/>
-      <c r="V63" s="9"/>
-      <c r="W63" s="9"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="5"/>
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="5"/>
+      <c r="Z63" s="5"/>
+      <c r="AA63" s="5"/>
+      <c r="AB63" s="8"/>
+      <c r="AC63" s="9"/>
+      <c r="AD63" s="9"/>
+      <c r="AE63" s="9"/>
+      <c r="AF63" s="9"/>
+      <c r="AG63" s="9"/>
+      <c r="AH63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5"/>
@@ -2560,13 +3371,24 @@
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
-      <c r="Q64" s="8"/>
-      <c r="R64" s="9"/>
-      <c r="S64" s="9"/>
-      <c r="T64" s="9"/>
-      <c r="U64" s="9"/>
-      <c r="V64" s="9"/>
-      <c r="W64" s="9"/>
+      <c r="Q64" s="5"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="5"/>
+      <c r="V64" s="5"/>
+      <c r="W64" s="5"/>
+      <c r="X64" s="5"/>
+      <c r="Y64" s="5"/>
+      <c r="Z64" s="5"/>
+      <c r="AA64" s="5"/>
+      <c r="AB64" s="8"/>
+      <c r="AC64" s="9"/>
+      <c r="AD64" s="9"/>
+      <c r="AE64" s="9"/>
+      <c r="AF64" s="9"/>
+      <c r="AG64" s="9"/>
+      <c r="AH64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
@@ -2585,13 +3407,24 @@
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="9"/>
-      <c r="S65" s="9"/>
-      <c r="T65" s="9"/>
-      <c r="U65" s="9"/>
-      <c r="V65" s="9"/>
-      <c r="W65" s="9"/>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="T65" s="5"/>
+      <c r="U65" s="5"/>
+      <c r="V65" s="5"/>
+      <c r="W65" s="5"/>
+      <c r="X65" s="5"/>
+      <c r="Y65" s="5"/>
+      <c r="Z65" s="5"/>
+      <c r="AA65" s="5"/>
+      <c r="AB65" s="8"/>
+      <c r="AC65" s="9"/>
+      <c r="AD65" s="9"/>
+      <c r="AE65" s="9"/>
+      <c r="AF65" s="9"/>
+      <c r="AG65" s="9"/>
+      <c r="AH65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
@@ -2610,13 +3443,24 @@
       <c r="N66" s="5"/>
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="9"/>
-      <c r="S66" s="9"/>
-      <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-      <c r="V66" s="9"/>
-      <c r="W66" s="9"/>
+      <c r="Q66" s="5"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="5"/>
+      <c r="V66" s="5"/>
+      <c r="W66" s="5"/>
+      <c r="X66" s="5"/>
+      <c r="Y66" s="5"/>
+      <c r="Z66" s="5"/>
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="8"/>
+      <c r="AC66" s="9"/>
+      <c r="AD66" s="9"/>
+      <c r="AE66" s="9"/>
+      <c r="AF66" s="9"/>
+      <c r="AG66" s="9"/>
+      <c r="AH66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5"/>
@@ -2635,13 +3479,24 @@
       <c r="N67" s="5"/>
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
-      <c r="Q67" s="8"/>
-      <c r="R67" s="9"/>
-      <c r="S67" s="9"/>
-      <c r="T67" s="9"/>
-      <c r="U67" s="9"/>
-      <c r="V67" s="9"/>
-      <c r="W67" s="9"/>
+      <c r="Q67" s="5"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="5"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="5"/>
+      <c r="V67" s="5"/>
+      <c r="W67" s="5"/>
+      <c r="X67" s="5"/>
+      <c r="Y67" s="5"/>
+      <c r="Z67" s="5"/>
+      <c r="AA67" s="5"/>
+      <c r="AB67" s="8"/>
+      <c r="AC67" s="9"/>
+      <c r="AD67" s="9"/>
+      <c r="AE67" s="9"/>
+      <c r="AF67" s="9"/>
+      <c r="AG67" s="9"/>
+      <c r="AH67" s="9"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5"/>
@@ -2660,13 +3515,24 @@
       <c r="N68" s="5"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="9"/>
-      <c r="S68" s="9"/>
-      <c r="T68" s="9"/>
-      <c r="U68" s="9"/>
-      <c r="V68" s="9"/>
-      <c r="W68" s="9"/>
+      <c r="Q68" s="5"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="5"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="5"/>
+      <c r="V68" s="5"/>
+      <c r="W68" s="5"/>
+      <c r="X68" s="5"/>
+      <c r="Y68" s="5"/>
+      <c r="Z68" s="5"/>
+      <c r="AA68" s="5"/>
+      <c r="AB68" s="8"/>
+      <c r="AC68" s="9"/>
+      <c r="AD68" s="9"/>
+      <c r="AE68" s="9"/>
+      <c r="AF68" s="9"/>
+      <c r="AG68" s="9"/>
+      <c r="AH68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5"/>
@@ -2685,13 +3551,24 @@
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
-      <c r="Q69" s="8"/>
-      <c r="R69" s="9"/>
-      <c r="S69" s="9"/>
-      <c r="T69" s="9"/>
-      <c r="U69" s="9"/>
-      <c r="V69" s="9"/>
-      <c r="W69" s="9"/>
+      <c r="Q69" s="5"/>
+      <c r="R69" s="5"/>
+      <c r="S69" s="5"/>
+      <c r="T69" s="5"/>
+      <c r="U69" s="5"/>
+      <c r="V69" s="5"/>
+      <c r="W69" s="5"/>
+      <c r="X69" s="5"/>
+      <c r="Y69" s="5"/>
+      <c r="Z69" s="5"/>
+      <c r="AA69" s="5"/>
+      <c r="AB69" s="8"/>
+      <c r="AC69" s="9"/>
+      <c r="AD69" s="9"/>
+      <c r="AE69" s="9"/>
+      <c r="AF69" s="9"/>
+      <c r="AG69" s="9"/>
+      <c r="AH69" s="9"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5"/>
@@ -2710,13 +3587,24 @@
       <c r="N70" s="5"/>
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="9"/>
-      <c r="S70" s="9"/>
-      <c r="T70" s="9"/>
-      <c r="U70" s="9"/>
-      <c r="V70" s="9"/>
-      <c r="W70" s="9"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="5"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="5"/>
+      <c r="X70" s="5"/>
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5"/>
+      <c r="AA70" s="5"/>
+      <c r="AB70" s="8"/>
+      <c r="AC70" s="9"/>
+      <c r="AD70" s="9"/>
+      <c r="AE70" s="9"/>
+      <c r="AF70" s="9"/>
+      <c r="AG70" s="9"/>
+      <c r="AH70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5"/>
@@ -2735,13 +3623,24 @@
       <c r="N71" s="5"/>
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="9"/>
-      <c r="S71" s="9"/>
-      <c r="T71" s="9"/>
-      <c r="U71" s="9"/>
-      <c r="V71" s="9"/>
-      <c r="W71" s="9"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="5"/>
+      <c r="S71" s="5"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="5"/>
+      <c r="V71" s="5"/>
+      <c r="W71" s="5"/>
+      <c r="X71" s="5"/>
+      <c r="Y71" s="5"/>
+      <c r="Z71" s="5"/>
+      <c r="AA71" s="5"/>
+      <c r="AB71" s="8"/>
+      <c r="AC71" s="9"/>
+      <c r="AD71" s="9"/>
+      <c r="AE71" s="9"/>
+      <c r="AF71" s="9"/>
+      <c r="AG71" s="9"/>
+      <c r="AH71" s="9"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5"/>
@@ -2760,13 +3659,24 @@
       <c r="N72" s="5"/>
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="9"/>
-      <c r="S72" s="9"/>
-      <c r="T72" s="9"/>
-      <c r="U72" s="9"/>
-      <c r="V72" s="9"/>
-      <c r="W72" s="9"/>
+      <c r="Q72" s="5"/>
+      <c r="R72" s="5"/>
+      <c r="S72" s="5"/>
+      <c r="T72" s="5"/>
+      <c r="U72" s="5"/>
+      <c r="V72" s="5"/>
+      <c r="W72" s="5"/>
+      <c r="X72" s="5"/>
+      <c r="Y72" s="5"/>
+      <c r="Z72" s="5"/>
+      <c r="AA72" s="5"/>
+      <c r="AB72" s="8"/>
+      <c r="AC72" s="9"/>
+      <c r="AD72" s="9"/>
+      <c r="AE72" s="9"/>
+      <c r="AF72" s="9"/>
+      <c r="AG72" s="9"/>
+      <c r="AH72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5"/>
@@ -2785,13 +3695,24 @@
       <c r="N73" s="5"/>
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="9"/>
-      <c r="S73" s="9"/>
-      <c r="T73" s="9"/>
-      <c r="U73" s="9"/>
-      <c r="V73" s="9"/>
-      <c r="W73" s="9"/>
+      <c r="Q73" s="5"/>
+      <c r="R73" s="5"/>
+      <c r="S73" s="5"/>
+      <c r="T73" s="5"/>
+      <c r="U73" s="5"/>
+      <c r="V73" s="5"/>
+      <c r="W73" s="5"/>
+      <c r="X73" s="5"/>
+      <c r="Y73" s="5"/>
+      <c r="Z73" s="5"/>
+      <c r="AA73" s="5"/>
+      <c r="AB73" s="8"/>
+      <c r="AC73" s="9"/>
+      <c r="AD73" s="9"/>
+      <c r="AE73" s="9"/>
+      <c r="AF73" s="9"/>
+      <c r="AG73" s="9"/>
+      <c r="AH73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5"/>
@@ -2810,13 +3731,24 @@
       <c r="N74" s="5"/>
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
-      <c r="Q74" s="8"/>
-      <c r="R74" s="9"/>
-      <c r="S74" s="9"/>
-      <c r="T74" s="9"/>
-      <c r="U74" s="9"/>
-      <c r="V74" s="9"/>
-      <c r="W74" s="9"/>
+      <c r="Q74" s="5"/>
+      <c r="R74" s="5"/>
+      <c r="S74" s="5"/>
+      <c r="T74" s="5"/>
+      <c r="U74" s="5"/>
+      <c r="V74" s="5"/>
+      <c r="W74" s="5"/>
+      <c r="X74" s="5"/>
+      <c r="Y74" s="5"/>
+      <c r="Z74" s="5"/>
+      <c r="AA74" s="5"/>
+      <c r="AB74" s="8"/>
+      <c r="AC74" s="9"/>
+      <c r="AD74" s="9"/>
+      <c r="AE74" s="9"/>
+      <c r="AF74" s="9"/>
+      <c r="AG74" s="9"/>
+      <c r="AH74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5"/>
@@ -2835,13 +3767,24 @@
       <c r="N75" s="5"/>
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
-      <c r="Q75" s="8"/>
-      <c r="R75" s="9"/>
-      <c r="S75" s="9"/>
-      <c r="T75" s="9"/>
-      <c r="U75" s="9"/>
-      <c r="V75" s="9"/>
-      <c r="W75" s="9"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5"/>
+      <c r="V75" s="5"/>
+      <c r="W75" s="5"/>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="5"/>
+      <c r="AA75" s="5"/>
+      <c r="AB75" s="8"/>
+      <c r="AC75" s="9"/>
+      <c r="AD75" s="9"/>
+      <c r="AE75" s="9"/>
+      <c r="AF75" s="9"/>
+      <c r="AG75" s="9"/>
+      <c r="AH75" s="9"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5"/>
@@ -2860,13 +3803,24 @@
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
-      <c r="Q76" s="8"/>
-      <c r="R76" s="9"/>
-      <c r="S76" s="9"/>
-      <c r="T76" s="9"/>
-      <c r="U76" s="9"/>
-      <c r="V76" s="9"/>
-      <c r="W76" s="9"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5"/>
+      <c r="V76" s="5"/>
+      <c r="W76" s="5"/>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5"/>
+      <c r="Z76" s="5"/>
+      <c r="AA76" s="5"/>
+      <c r="AB76" s="8"/>
+      <c r="AC76" s="9"/>
+      <c r="AD76" s="9"/>
+      <c r="AE76" s="9"/>
+      <c r="AF76" s="9"/>
+      <c r="AG76" s="9"/>
+      <c r="AH76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5"/>
@@ -2885,13 +3839,24 @@
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="9"/>
-      <c r="S77" s="9"/>
-      <c r="T77" s="9"/>
-      <c r="U77" s="9"/>
-      <c r="V77" s="9"/>
-      <c r="W77" s="9"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5"/>
+      <c r="V77" s="5"/>
+      <c r="W77" s="5"/>
+      <c r="X77" s="5"/>
+      <c r="Y77" s="5"/>
+      <c r="Z77" s="5"/>
+      <c r="AA77" s="5"/>
+      <c r="AB77" s="8"/>
+      <c r="AC77" s="9"/>
+      <c r="AD77" s="9"/>
+      <c r="AE77" s="9"/>
+      <c r="AF77" s="9"/>
+      <c r="AG77" s="9"/>
+      <c r="AH77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5"/>
@@ -2910,13 +3875,24 @@
       <c r="N78" s="5"/>
       <c r="O78" s="5"/>
       <c r="P78" s="5"/>
-      <c r="Q78" s="8"/>
-      <c r="R78" s="9"/>
-      <c r="S78" s="9"/>
-      <c r="T78" s="9"/>
-      <c r="U78" s="9"/>
-      <c r="V78" s="9"/>
-      <c r="W78" s="9"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="T78" s="5"/>
+      <c r="U78" s="5"/>
+      <c r="V78" s="5"/>
+      <c r="W78" s="5"/>
+      <c r="X78" s="5"/>
+      <c r="Y78" s="5"/>
+      <c r="Z78" s="5"/>
+      <c r="AA78" s="5"/>
+      <c r="AB78" s="8"/>
+      <c r="AC78" s="9"/>
+      <c r="AD78" s="9"/>
+      <c r="AE78" s="9"/>
+      <c r="AF78" s="9"/>
+      <c r="AG78" s="9"/>
+      <c r="AH78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5"/>
@@ -2935,13 +3911,24 @@
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
       <c r="P79" s="5"/>
-      <c r="Q79" s="8"/>
-      <c r="R79" s="9"/>
-      <c r="S79" s="9"/>
-      <c r="T79" s="9"/>
-      <c r="U79" s="9"/>
-      <c r="V79" s="9"/>
-      <c r="W79" s="9"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="V79" s="5"/>
+      <c r="W79" s="5"/>
+      <c r="X79" s="5"/>
+      <c r="Y79" s="5"/>
+      <c r="Z79" s="5"/>
+      <c r="AA79" s="5"/>
+      <c r="AB79" s="8"/>
+      <c r="AC79" s="9"/>
+      <c r="AD79" s="9"/>
+      <c r="AE79" s="9"/>
+      <c r="AF79" s="9"/>
+      <c r="AG79" s="9"/>
+      <c r="AH79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5"/>
@@ -2960,13 +3947,24 @@
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
       <c r="P80" s="5"/>
-      <c r="Q80" s="8"/>
-      <c r="R80" s="9"/>
-      <c r="S80" s="9"/>
-      <c r="T80" s="9"/>
-      <c r="U80" s="9"/>
-      <c r="V80" s="9"/>
-      <c r="W80" s="9"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5"/>
+      <c r="U80" s="5"/>
+      <c r="V80" s="5"/>
+      <c r="W80" s="5"/>
+      <c r="X80" s="5"/>
+      <c r="Y80" s="5"/>
+      <c r="Z80" s="5"/>
+      <c r="AA80" s="5"/>
+      <c r="AB80" s="8"/>
+      <c r="AC80" s="9"/>
+      <c r="AD80" s="9"/>
+      <c r="AE80" s="9"/>
+      <c r="AF80" s="9"/>
+      <c r="AG80" s="9"/>
+      <c r="AH80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5"/>
@@ -2985,13 +3983,24 @@
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
       <c r="P81" s="5"/>
-      <c r="Q81" s="8"/>
-      <c r="R81" s="9"/>
-      <c r="S81" s="9"/>
-      <c r="T81" s="9"/>
-      <c r="U81" s="9"/>
-      <c r="V81" s="9"/>
-      <c r="W81" s="9"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5"/>
+      <c r="U81" s="5"/>
+      <c r="V81" s="5"/>
+      <c r="W81" s="5"/>
+      <c r="X81" s="5"/>
+      <c r="Y81" s="5"/>
+      <c r="Z81" s="5"/>
+      <c r="AA81" s="5"/>
+      <c r="AB81" s="8"/>
+      <c r="AC81" s="9"/>
+      <c r="AD81" s="9"/>
+      <c r="AE81" s="9"/>
+      <c r="AF81" s="9"/>
+      <c r="AG81" s="9"/>
+      <c r="AH81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5"/>
@@ -3010,13 +4019,24 @@
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
       <c r="P82" s="5"/>
-      <c r="Q82" s="8"/>
-      <c r="R82" s="9"/>
-      <c r="S82" s="9"/>
-      <c r="T82" s="9"/>
-      <c r="U82" s="9"/>
-      <c r="V82" s="9"/>
-      <c r="W82" s="9"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5"/>
+      <c r="U82" s="5"/>
+      <c r="V82" s="5"/>
+      <c r="W82" s="5"/>
+      <c r="X82" s="5"/>
+      <c r="Y82" s="5"/>
+      <c r="Z82" s="5"/>
+      <c r="AA82" s="5"/>
+      <c r="AB82" s="8"/>
+      <c r="AC82" s="9"/>
+      <c r="AD82" s="9"/>
+      <c r="AE82" s="9"/>
+      <c r="AF82" s="9"/>
+      <c r="AG82" s="9"/>
+      <c r="AH82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5"/>
@@ -3035,13 +4055,24 @@
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
       <c r="P83" s="5"/>
-      <c r="Q83" s="8"/>
-      <c r="R83" s="9"/>
-      <c r="S83" s="9"/>
-      <c r="T83" s="9"/>
-      <c r="U83" s="9"/>
-      <c r="V83" s="9"/>
-      <c r="W83" s="9"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5"/>
+      <c r="U83" s="5"/>
+      <c r="V83" s="5"/>
+      <c r="W83" s="5"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5"/>
+      <c r="AA83" s="5"/>
+      <c r="AB83" s="8"/>
+      <c r="AC83" s="9"/>
+      <c r="AD83" s="9"/>
+      <c r="AE83" s="9"/>
+      <c r="AF83" s="9"/>
+      <c r="AG83" s="9"/>
+      <c r="AH83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5"/>
@@ -3060,13 +4091,24 @@
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
       <c r="P84" s="5"/>
-      <c r="Q84" s="8"/>
-      <c r="R84" s="9"/>
-      <c r="S84" s="9"/>
-      <c r="T84" s="9"/>
-      <c r="U84" s="9"/>
-      <c r="V84" s="9"/>
-      <c r="W84" s="9"/>
+      <c r="Q84" s="5"/>
+      <c r="R84" s="5"/>
+      <c r="S84" s="5"/>
+      <c r="T84" s="5"/>
+      <c r="U84" s="5"/>
+      <c r="V84" s="5"/>
+      <c r="W84" s="5"/>
+      <c r="X84" s="5"/>
+      <c r="Y84" s="5"/>
+      <c r="Z84" s="5"/>
+      <c r="AA84" s="5"/>
+      <c r="AB84" s="8"/>
+      <c r="AC84" s="9"/>
+      <c r="AD84" s="9"/>
+      <c r="AE84" s="9"/>
+      <c r="AF84" s="9"/>
+      <c r="AG84" s="9"/>
+      <c r="AH84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5"/>
@@ -3085,13 +4127,24 @@
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
       <c r="P85" s="5"/>
-      <c r="Q85" s="8"/>
-      <c r="R85" s="9"/>
-      <c r="S85" s="9"/>
-      <c r="T85" s="9"/>
-      <c r="U85" s="9"/>
-      <c r="V85" s="9"/>
-      <c r="W85" s="9"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="T85" s="5"/>
+      <c r="U85" s="5"/>
+      <c r="V85" s="5"/>
+      <c r="W85" s="5"/>
+      <c r="X85" s="5"/>
+      <c r="Y85" s="5"/>
+      <c r="Z85" s="5"/>
+      <c r="AA85" s="5"/>
+      <c r="AB85" s="8"/>
+      <c r="AC85" s="9"/>
+      <c r="AD85" s="9"/>
+      <c r="AE85" s="9"/>
+      <c r="AF85" s="9"/>
+      <c r="AG85" s="9"/>
+      <c r="AH85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5"/>
@@ -3110,13 +4163,24 @@
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
       <c r="P86" s="5"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="9"/>
-      <c r="S86" s="9"/>
-      <c r="T86" s="9"/>
-      <c r="U86" s="9"/>
-      <c r="V86" s="9"/>
-      <c r="W86" s="9"/>
+      <c r="Q86" s="5"/>
+      <c r="R86" s="5"/>
+      <c r="S86" s="5"/>
+      <c r="T86" s="5"/>
+      <c r="U86" s="5"/>
+      <c r="V86" s="5"/>
+      <c r="W86" s="5"/>
+      <c r="X86" s="5"/>
+      <c r="Y86" s="5"/>
+      <c r="Z86" s="5"/>
+      <c r="AA86" s="5"/>
+      <c r="AB86" s="8"/>
+      <c r="AC86" s="9"/>
+      <c r="AD86" s="9"/>
+      <c r="AE86" s="9"/>
+      <c r="AF86" s="9"/>
+      <c r="AG86" s="9"/>
+      <c r="AH86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5"/>
@@ -3135,13 +4199,24 @@
       <c r="N87" s="5"/>
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
-      <c r="Q87" s="8"/>
-      <c r="R87" s="9"/>
-      <c r="S87" s="9"/>
-      <c r="T87" s="9"/>
-      <c r="U87" s="9"/>
-      <c r="V87" s="9"/>
-      <c r="W87" s="9"/>
+      <c r="Q87" s="5"/>
+      <c r="R87" s="5"/>
+      <c r="S87" s="5"/>
+      <c r="T87" s="5"/>
+      <c r="U87" s="5"/>
+      <c r="V87" s="5"/>
+      <c r="W87" s="5"/>
+      <c r="X87" s="5"/>
+      <c r="Y87" s="5"/>
+      <c r="Z87" s="5"/>
+      <c r="AA87" s="5"/>
+      <c r="AB87" s="8"/>
+      <c r="AC87" s="9"/>
+      <c r="AD87" s="9"/>
+      <c r="AE87" s="9"/>
+      <c r="AF87" s="9"/>
+      <c r="AG87" s="9"/>
+      <c r="AH87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5"/>
@@ -3160,13 +4235,24 @@
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
-      <c r="Q88" s="8"/>
-      <c r="R88" s="9"/>
-      <c r="S88" s="9"/>
-      <c r="T88" s="9"/>
-      <c r="U88" s="9"/>
-      <c r="V88" s="9"/>
-      <c r="W88" s="9"/>
+      <c r="Q88" s="5"/>
+      <c r="R88" s="5"/>
+      <c r="S88" s="5"/>
+      <c r="T88" s="5"/>
+      <c r="U88" s="5"/>
+      <c r="V88" s="5"/>
+      <c r="W88" s="5"/>
+      <c r="X88" s="5"/>
+      <c r="Y88" s="5"/>
+      <c r="Z88" s="5"/>
+      <c r="AA88" s="5"/>
+      <c r="AB88" s="8"/>
+      <c r="AC88" s="9"/>
+      <c r="AD88" s="9"/>
+      <c r="AE88" s="9"/>
+      <c r="AF88" s="9"/>
+      <c r="AG88" s="9"/>
+      <c r="AH88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5"/>
@@ -3185,13 +4271,24 @@
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
-      <c r="Q89" s="8"/>
-      <c r="R89" s="9"/>
-      <c r="S89" s="9"/>
-      <c r="T89" s="9"/>
-      <c r="U89" s="9"/>
-      <c r="V89" s="9"/>
-      <c r="W89" s="9"/>
+      <c r="Q89" s="5"/>
+      <c r="R89" s="5"/>
+      <c r="S89" s="5"/>
+      <c r="T89" s="5"/>
+      <c r="U89" s="5"/>
+      <c r="V89" s="5"/>
+      <c r="W89" s="5"/>
+      <c r="X89" s="5"/>
+      <c r="Y89" s="5"/>
+      <c r="Z89" s="5"/>
+      <c r="AA89" s="5"/>
+      <c r="AB89" s="8"/>
+      <c r="AC89" s="9"/>
+      <c r="AD89" s="9"/>
+      <c r="AE89" s="9"/>
+      <c r="AF89" s="9"/>
+      <c r="AG89" s="9"/>
+      <c r="AH89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5"/>
@@ -3210,13 +4307,24 @@
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="9"/>
-      <c r="S90" s="9"/>
-      <c r="T90" s="9"/>
-      <c r="U90" s="9"/>
-      <c r="V90" s="9"/>
-      <c r="W90" s="9"/>
+      <c r="Q90" s="5"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="5"/>
+      <c r="T90" s="5"/>
+      <c r="U90" s="5"/>
+      <c r="V90" s="5"/>
+      <c r="W90" s="5"/>
+      <c r="X90" s="5"/>
+      <c r="Y90" s="5"/>
+      <c r="Z90" s="5"/>
+      <c r="AA90" s="5"/>
+      <c r="AB90" s="8"/>
+      <c r="AC90" s="9"/>
+      <c r="AD90" s="9"/>
+      <c r="AE90" s="9"/>
+      <c r="AF90" s="9"/>
+      <c r="AG90" s="9"/>
+      <c r="AH90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5"/>
@@ -3235,13 +4343,24 @@
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
       <c r="P91" s="5"/>
-      <c r="Q91" s="8"/>
-      <c r="R91" s="9"/>
-      <c r="S91" s="9"/>
-      <c r="T91" s="9"/>
-      <c r="U91" s="9"/>
-      <c r="V91" s="9"/>
-      <c r="W91" s="9"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+      <c r="T91" s="5"/>
+      <c r="U91" s="5"/>
+      <c r="V91" s="5"/>
+      <c r="W91" s="5"/>
+      <c r="X91" s="5"/>
+      <c r="Y91" s="5"/>
+      <c r="Z91" s="5"/>
+      <c r="AA91" s="5"/>
+      <c r="AB91" s="8"/>
+      <c r="AC91" s="9"/>
+      <c r="AD91" s="9"/>
+      <c r="AE91" s="9"/>
+      <c r="AF91" s="9"/>
+      <c r="AG91" s="9"/>
+      <c r="AH91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5"/>
@@ -3260,13 +4379,24 @@
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
       <c r="P92" s="5"/>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="9"/>
-      <c r="S92" s="9"/>
-      <c r="T92" s="9"/>
-      <c r="U92" s="9"/>
-      <c r="V92" s="9"/>
-      <c r="W92" s="9"/>
+      <c r="Q92" s="5"/>
+      <c r="R92" s="5"/>
+      <c r="S92" s="5"/>
+      <c r="T92" s="5"/>
+      <c r="U92" s="5"/>
+      <c r="V92" s="5"/>
+      <c r="W92" s="5"/>
+      <c r="X92" s="5"/>
+      <c r="Y92" s="5"/>
+      <c r="Z92" s="5"/>
+      <c r="AA92" s="5"/>
+      <c r="AB92" s="8"/>
+      <c r="AC92" s="9"/>
+      <c r="AD92" s="9"/>
+      <c r="AE92" s="9"/>
+      <c r="AF92" s="9"/>
+      <c r="AG92" s="9"/>
+      <c r="AH92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5"/>
@@ -3285,13 +4415,24 @@
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
       <c r="P93" s="5"/>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="9"/>
-      <c r="S93" s="9"/>
-      <c r="T93" s="9"/>
-      <c r="U93" s="9"/>
-      <c r="V93" s="9"/>
-      <c r="W93" s="9"/>
+      <c r="Q93" s="5"/>
+      <c r="R93" s="5"/>
+      <c r="S93" s="5"/>
+      <c r="T93" s="5"/>
+      <c r="U93" s="5"/>
+      <c r="V93" s="5"/>
+      <c r="W93" s="5"/>
+      <c r="X93" s="5"/>
+      <c r="Y93" s="5"/>
+      <c r="Z93" s="5"/>
+      <c r="AA93" s="5"/>
+      <c r="AB93" s="8"/>
+      <c r="AC93" s="9"/>
+      <c r="AD93" s="9"/>
+      <c r="AE93" s="9"/>
+      <c r="AF93" s="9"/>
+      <c r="AG93" s="9"/>
+      <c r="AH93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5"/>
@@ -3310,13 +4451,24 @@
       <c r="N94" s="5"/>
       <c r="O94" s="5"/>
       <c r="P94" s="5"/>
-      <c r="Q94" s="8"/>
-      <c r="R94" s="9"/>
-      <c r="S94" s="9"/>
-      <c r="T94" s="9"/>
-      <c r="U94" s="9"/>
-      <c r="V94" s="9"/>
-      <c r="W94" s="9"/>
+      <c r="Q94" s="5"/>
+      <c r="R94" s="5"/>
+      <c r="S94" s="5"/>
+      <c r="T94" s="5"/>
+      <c r="U94" s="5"/>
+      <c r="V94" s="5"/>
+      <c r="W94" s="5"/>
+      <c r="X94" s="5"/>
+      <c r="Y94" s="5"/>
+      <c r="Z94" s="5"/>
+      <c r="AA94" s="5"/>
+      <c r="AB94" s="8"/>
+      <c r="AC94" s="9"/>
+      <c r="AD94" s="9"/>
+      <c r="AE94" s="9"/>
+      <c r="AF94" s="9"/>
+      <c r="AG94" s="9"/>
+      <c r="AH94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5"/>
@@ -3335,13 +4487,24 @@
       <c r="N95" s="5"/>
       <c r="O95" s="5"/>
       <c r="P95" s="5"/>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="9"/>
-      <c r="S95" s="9"/>
-      <c r="T95" s="9"/>
-      <c r="U95" s="9"/>
-      <c r="V95" s="9"/>
-      <c r="W95" s="9"/>
+      <c r="Q95" s="5"/>
+      <c r="R95" s="5"/>
+      <c r="S95" s="5"/>
+      <c r="T95" s="5"/>
+      <c r="U95" s="5"/>
+      <c r="V95" s="5"/>
+      <c r="W95" s="5"/>
+      <c r="X95" s="5"/>
+      <c r="Y95" s="5"/>
+      <c r="Z95" s="5"/>
+      <c r="AA95" s="5"/>
+      <c r="AB95" s="8"/>
+      <c r="AC95" s="9"/>
+      <c r="AD95" s="9"/>
+      <c r="AE95" s="9"/>
+      <c r="AF95" s="9"/>
+      <c r="AG95" s="9"/>
+      <c r="AH95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5"/>
@@ -3360,13 +4523,24 @@
       <c r="N96" s="5"/>
       <c r="O96" s="5"/>
       <c r="P96" s="5"/>
-      <c r="Q96" s="8"/>
-      <c r="R96" s="9"/>
-      <c r="S96" s="9"/>
-      <c r="T96" s="9"/>
-      <c r="U96" s="9"/>
-      <c r="V96" s="9"/>
-      <c r="W96" s="9"/>
+      <c r="Q96" s="5"/>
+      <c r="R96" s="5"/>
+      <c r="S96" s="5"/>
+      <c r="T96" s="5"/>
+      <c r="U96" s="5"/>
+      <c r="V96" s="5"/>
+      <c r="W96" s="5"/>
+      <c r="X96" s="5"/>
+      <c r="Y96" s="5"/>
+      <c r="Z96" s="5"/>
+      <c r="AA96" s="5"/>
+      <c r="AB96" s="8"/>
+      <c r="AC96" s="9"/>
+      <c r="AD96" s="9"/>
+      <c r="AE96" s="9"/>
+      <c r="AF96" s="9"/>
+      <c r="AG96" s="9"/>
+      <c r="AH96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5"/>
@@ -3385,13 +4559,24 @@
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
       <c r="P97" s="5"/>
-      <c r="Q97" s="8"/>
-      <c r="R97" s="9"/>
-      <c r="S97" s="9"/>
-      <c r="T97" s="9"/>
-      <c r="U97" s="9"/>
-      <c r="V97" s="9"/>
-      <c r="W97" s="9"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
+      <c r="Y97" s="5"/>
+      <c r="Z97" s="5"/>
+      <c r="AA97" s="5"/>
+      <c r="AB97" s="8"/>
+      <c r="AC97" s="9"/>
+      <c r="AD97" s="9"/>
+      <c r="AE97" s="9"/>
+      <c r="AF97" s="9"/>
+      <c r="AG97" s="9"/>
+      <c r="AH97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5"/>
@@ -3410,13 +4595,24 @@
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
       <c r="P98" s="5"/>
-      <c r="Q98" s="8"/>
-      <c r="R98" s="9"/>
-      <c r="S98" s="9"/>
-      <c r="T98" s="9"/>
-      <c r="U98" s="9"/>
-      <c r="V98" s="9"/>
-      <c r="W98" s="9"/>
+      <c r="Q98" s="5"/>
+      <c r="R98" s="5"/>
+      <c r="S98" s="5"/>
+      <c r="T98" s="5"/>
+      <c r="U98" s="5"/>
+      <c r="V98" s="5"/>
+      <c r="W98" s="5"/>
+      <c r="X98" s="5"/>
+      <c r="Y98" s="5"/>
+      <c r="Z98" s="5"/>
+      <c r="AA98" s="5"/>
+      <c r="AB98" s="8"/>
+      <c r="AC98" s="9"/>
+      <c r="AD98" s="9"/>
+      <c r="AE98" s="9"/>
+      <c r="AF98" s="9"/>
+      <c r="AG98" s="9"/>
+      <c r="AH98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5"/>
@@ -3435,13 +4631,24 @@
       <c r="N99" s="5"/>
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
-      <c r="Q99" s="8"/>
-      <c r="R99" s="9"/>
-      <c r="S99" s="9"/>
-      <c r="T99" s="9"/>
-      <c r="U99" s="9"/>
-      <c r="V99" s="9"/>
-      <c r="W99" s="9"/>
+      <c r="Q99" s="5"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="5"/>
+      <c r="T99" s="5"/>
+      <c r="U99" s="5"/>
+      <c r="V99" s="5"/>
+      <c r="W99" s="5"/>
+      <c r="X99" s="5"/>
+      <c r="Y99" s="5"/>
+      <c r="Z99" s="5"/>
+      <c r="AA99" s="5"/>
+      <c r="AB99" s="8"/>
+      <c r="AC99" s="9"/>
+      <c r="AD99" s="9"/>
+      <c r="AE99" s="9"/>
+      <c r="AF99" s="9"/>
+      <c r="AG99" s="9"/>
+      <c r="AH99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5"/>
@@ -3460,13 +4667,24 @@
       <c r="N100" s="5"/>
       <c r="O100" s="5"/>
       <c r="P100" s="5"/>
-      <c r="Q100" s="8"/>
-      <c r="R100" s="9"/>
-      <c r="S100" s="9"/>
-      <c r="T100" s="9"/>
-      <c r="U100" s="9"/>
-      <c r="V100" s="9"/>
-      <c r="W100" s="9"/>
+      <c r="Q100" s="5"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="5"/>
+      <c r="T100" s="5"/>
+      <c r="U100" s="5"/>
+      <c r="V100" s="5"/>
+      <c r="W100" s="5"/>
+      <c r="X100" s="5"/>
+      <c r="Y100" s="5"/>
+      <c r="Z100" s="5"/>
+      <c r="AA100" s="5"/>
+      <c r="AB100" s="8"/>
+      <c r="AC100" s="9"/>
+      <c r="AD100" s="9"/>
+      <c r="AE100" s="9"/>
+      <c r="AF100" s="9"/>
+      <c r="AG100" s="9"/>
+      <c r="AH100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="13"/>
@@ -3485,13 +4703,24 @@
       <c r="N101" s="5"/>
       <c r="O101" s="13"/>
       <c r="P101" s="13"/>
-      <c r="Q101" s="14"/>
-      <c r="R101" s="15"/>
-      <c r="S101" s="15"/>
-      <c r="T101" s="15"/>
-      <c r="U101" s="15"/>
-      <c r="V101" s="15"/>
-      <c r="W101" s="15"/>
+      <c r="Q101" s="13"/>
+      <c r="R101" s="13"/>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+      <c r="U101" s="13"/>
+      <c r="V101" s="13"/>
+      <c r="W101" s="13"/>
+      <c r="X101" s="13"/>
+      <c r="Y101" s="13"/>
+      <c r="Z101" s="13"/>
+      <c r="AA101" s="13"/>
+      <c r="AB101" s="14"/>
+      <c r="AC101" s="15"/>
+      <c r="AD101" s="15"/>
+      <c r="AE101" s="15"/>
+      <c r="AF101" s="15"/>
+      <c r="AG101" s="15"/>
+      <c r="AH101" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
visszautasas sablon plusz excel int float baszodas fix
</commit_message>
<xml_diff>
--- a/contracts-list.xlsx
+++ b/contracts-list.xlsx
@@ -443,6 +443,7 @@
       <color rgb="FF000000"/>
       <name val="Garamond"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -778,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB4" activeCellId="0" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -795,7 +796,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="26.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="19" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="21" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="25" style="0" width="23.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="38.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="16.31"/>
@@ -858,10 +862,10 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
@@ -873,7 +877,7 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="3" t="s">
@@ -908,7 +912,7 @@
       </c>
       <c r="AI1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -962,10 +966,10 @@
         <v>48</v>
       </c>
       <c r="S2" s="5" t="n">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="T2" s="5" t="n">
-        <v>5463</v>
+        <v>43533</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>49</v>
@@ -1064,12 +1068,18 @@
       <c r="R3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="S3" s="5" t="n">
+        <v>1112</v>
+      </c>
+      <c r="T3" s="5" t="n">
+        <v>43534</v>
+      </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
+      <c r="X3" s="5" t="n">
+        <v>12</v>
+      </c>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -1149,12 +1159,18 @@
       <c r="R4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="S4" s="5" t="n">
+        <v>1113</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>43535</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
+      <c r="X4" s="5" t="n">
+        <v>13</v>
+      </c>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
@@ -1234,12 +1250,18 @@
       <c r="R5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="S5" s="5" t="n">
+        <v>1114</v>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>43536</v>
+      </c>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
+      <c r="X5" s="5" t="n">
+        <v>14</v>
+      </c>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
@@ -1319,12 +1341,18 @@
       <c r="R6" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="S6" s="5" t="n">
+        <v>1115</v>
+      </c>
+      <c r="T6" s="5" t="n">
+        <v>11415</v>
+      </c>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
+      <c r="X6" s="5" t="n">
+        <v>15</v>
+      </c>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>

</xml_diff>